<commit_message>
story:347 Generate UUT list based on os type
</commit_message>
<xml_diff>
--- a/Test_Plan/TEST_PLAN_2.xlsx
+++ b/Test_Plan/TEST_PLAN_2.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\Automation-Framework\Test_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDC8F8A-F309-407C-94E1-B0B31B49331C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5240CBF-C852-40AA-82CA-122574C8F988}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32256" yWindow="3456" windowWidth="18660" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix bug "if 'wes' in i.get_version.lower():" update testplan2 with usable test unit
</commit_message>
<xml_diff>
--- a/Test_Plan/TEST_PLAN_2.xlsx
+++ b/Test_Plan/TEST_PLAN_2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\Automation-Framework\Test_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panba\Desktop\work\work_projects\automation_20191008\Test_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5240CBF-C852-40AA-82CA-122574C8F988}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4629ADA-0937-4B3B-B01A-A74A673FDDED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="32256" yWindow="3456" windowWidth="18660" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,12 @@
     <t>name</t>
   </si>
   <si>
+    <t>Automation_demo</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
-    <t>balance.cheng@hp.com</t>
-  </si>
-  <si>
     <t>needbuild</t>
   </si>
   <si>
@@ -61,12 +61,6 @@
     <t>OS</t>
   </si>
   <si>
-    <t>15.83.250.20</t>
-  </si>
-  <si>
-    <t>48:0F:CF:BC:DD:3C</t>
-  </si>
-  <si>
     <t>WES10</t>
   </si>
   <si>
@@ -94,6 +88,15 @@
     <t>Doraemon</t>
   </si>
   <si>
+    <t>print_hello</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>check_basic_info</t>
+  </si>
+  <si>
     <t>script3</t>
   </si>
   <si>
@@ -106,16 +109,13 @@
     <t>script6</t>
   </si>
   <si>
-    <t>print_hello</t>
-  </si>
-  <si>
-    <t>check_basic_info</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Automation_demo</t>
+    <t>15.83.248.212</t>
+  </si>
+  <si>
+    <t>DC:4A:3E:04:A9:83</t>
+  </si>
+  <si>
+    <t>balance.cheng@hp.com;bamboo.pan@hp.com</t>
   </si>
 </sst>
 </file>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,15 +531,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,24 +603,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +642,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,79 +654,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>